<commit_message>
Set up a bit
</commit_message>
<xml_diff>
--- a/StudentManagementSystem/Sample data/Trainee_Import_Template.xlsx
+++ b/StudentManagementSystem/Sample data/Trainee_Import_Template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t xml:space="preserve">Họ và tên</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Tốt</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t xml:space="preserve">Nguyễn Văn Bố</t>
@@ -176,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -185,9 +188,6 @@
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -659,7 +659,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -679,7 +679,7 @@
     <col customWidth="1" min="12" max="12" style="1" width="29.69361686706543"/>
     <col customWidth="1" min="13" max="13" width="11.382844924926758"/>
     <col customWidth="1" min="14" max="14" width="20.722270965576172"/>
-    <col customWidth="1" min="15" max="15" width="9.5688982009887695"/>
+    <col customWidth="1" min="15" max="15" width="9.140625"/>
     <col customWidth="1" min="16" max="16" width="16.997797012329102"/>
     <col customWidth="1" min="17" max="17" width="16.679210662841797"/>
     <col customWidth="1" min="18" max="18" width="14.440144538879395"/>
@@ -792,22 +792,28 @@
       <c r="N2" t="s">
         <v>30</v>
       </c>
+      <c r="O2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
       <c r="Q2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="T2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" ht="15.75">
       <c r="A3" s="4" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>21</v>
@@ -851,20 +857,20 @@
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" ht="15.75">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -909,20 +915,20 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" ht="15.75">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -967,77 +973,79 @@
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" ht="15.75">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K6" t="s">
-        <v>25</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M6" t="s">
-        <v>29</v>
-      </c>
-      <c r="N6" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>31</v>
-      </c>
-      <c r="R6" t="s">
-        <v>32</v>
-      </c>
-      <c r="S6" t="s">
-        <v>33</v>
-      </c>
-      <c r="T6" t="s">
-        <v>34</v>
+      <c r="A6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="7" ht="15.75">
       <c r="A7" s="4" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>21</v>
@@ -1081,20 +1089,20 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" ht="15.75">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -1139,20 +1147,20 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="T8" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" ht="15.75">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -1197,77 +1205,79 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" ht="15.75">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" t="s">
-        <v>26</v>
-      </c>
-      <c r="I10" t="s">
-        <v>25</v>
-      </c>
-      <c r="J10" t="s">
-        <v>27</v>
-      </c>
-      <c r="K10" t="s">
-        <v>25</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M10" t="s">
-        <v>29</v>
-      </c>
-      <c r="N10" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>31</v>
-      </c>
-      <c r="R10" t="s">
-        <v>32</v>
-      </c>
-      <c r="S10" t="s">
-        <v>33</v>
-      </c>
-      <c r="T10" t="s">
-        <v>34</v>
+      <c r="A10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" ht="15.75">
       <c r="A11" s="4" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>21</v>
@@ -1311,20 +1321,20 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S11" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="T11" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" ht="15.75">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1369,20 +1379,20 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S12" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="T12" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" ht="15.75">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -1427,77 +1437,79 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S13" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="T13" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" ht="15.75">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J14" t="s">
-        <v>27</v>
-      </c>
-      <c r="K14" t="s">
-        <v>25</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M14" t="s">
-        <v>29</v>
-      </c>
-      <c r="N14" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>31</v>
-      </c>
-      <c r="R14" t="s">
-        <v>32</v>
-      </c>
-      <c r="S14" t="s">
-        <v>33</v>
-      </c>
-      <c r="T14" t="s">
-        <v>34</v>
+      <c r="A14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="15" ht="15.75">
       <c r="A15" s="4" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>21</v>
@@ -1541,20 +1553,20 @@
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S15" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="T15" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" ht="15.75">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -1599,20 +1611,20 @@
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="T16" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" ht="15.75">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -1657,77 +1669,79 @@
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R17" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S17" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="T17" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" ht="15.75">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" t="s">
-        <v>25</v>
-      </c>
-      <c r="H18" t="s">
-        <v>26</v>
-      </c>
-      <c r="I18" t="s">
-        <v>25</v>
-      </c>
-      <c r="J18" t="s">
-        <v>27</v>
-      </c>
-      <c r="K18" t="s">
-        <v>25</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M18" t="s">
-        <v>29</v>
-      </c>
-      <c r="N18" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>31</v>
-      </c>
-      <c r="R18" t="s">
-        <v>32</v>
-      </c>
-      <c r="S18" t="s">
-        <v>33</v>
-      </c>
-      <c r="T18" t="s">
-        <v>34</v>
+      <c r="A18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="R18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="S18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="T18" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="19" ht="15.75">
       <c r="A19" s="4" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>21</v>
@@ -1771,20 +1785,20 @@
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R19" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S19" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="T19" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" ht="15.75">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -1829,20 +1843,20 @@
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R20" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S20" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="T20" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" ht="15.75">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -1887,16 +1901,74 @@
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R21" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S21" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="T21" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" ht="15.75">
+      <c r="A22" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="S22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="T22" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>